<commit_message>
Agregar la hoja sd_cs
Para realizar la importación del archivo sd_cs.
</commit_message>
<xml_diff>
--- a/Tasas/Utils/Utils.xlsx
+++ b/Tasas/Utils/Utils.xlsx
@@ -10,6 +10,7 @@
     <sheet state="visible" name="import" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="df.factors" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="labels" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="sd_cs" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4289" uniqueCount="2026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4295" uniqueCount="2029">
   <si>
     <t>id</t>
   </si>
@@ -5485,7 +5486,7 @@
     <t>p4c</t>
   </si>
   <si>
-    <t xml:space="preserve">Pregunta 4c Entonces, ¿estamos hablando de que este negocio es _x0085_ </t>
+    <t>Pregunta 4c Entonces, ¿estamos hablando de que este negocio es _x0085_</t>
   </si>
   <si>
     <t>p4d1</t>
@@ -6094,7 +6095,16 @@
     <t>year</t>
   </si>
   <si>
-    <t>Año de levantamient</t>
+    <t>Año de levantamiento</t>
+  </si>
+  <si>
+    <t>p4d2_1</t>
+  </si>
+  <si>
+    <t>https://github.com/AlfCano/enoe/raw/devel/Tasas/Utils/meta_sd_cs.RData</t>
+  </si>
+  <si>
+    <t>sd.cs</t>
   </si>
 </sst>
 </file>
@@ -6182,6 +6192,10 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -18301,6 +18315,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="98.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -21303,6 +21320,48 @@
         <v>2025</v>
       </c>
     </row>
+    <row r="333">
+      <c r="A333" s="3" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B333" s="3" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>2027</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2028</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>